<commit_message>
modified:   data/Book_rank_title.xlsx 	new file:   data/ReviewsRankforAsins.csv 	new file:   data/reasonable_reviews.csv 	new file:   data/sortedRankAfterProcessed.csv
</commit_message>
<xml_diff>
--- a/data/Book_rank_title.xlsx
+++ b/data/Book_rank_title.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\shared_with_honey\NEU\cs5100 Foundation of Artificial intelligence\project\CS5100ProjectNew\CS5100Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FA9894-F7B2-4F5A-82B7-1D42C9B83F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7696664A-9929-4338-B44F-264FC7D35E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95E510F7-2AD1-41B5-8D35-BE3A425AE58B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95E510F7-2AD1-41B5-8D35-BE3A425AE58B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -797,9 +797,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,13 +1137,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7616D76E-44C9-4CA5-8577-213F12763658}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A85" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="115.5703125" customWidth="1"/>
     <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
@@ -1151,7 +1152,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B1" t="s">
@@ -1171,7 +1172,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1191,7 +1192,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -1211,7 +1212,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -1231,7 +1232,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5">
@@ -1251,7 +1252,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6">
@@ -1271,7 +1272,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>1419708457</v>
       </c>
       <c r="B7">
@@ -1291,7 +1292,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>1609580834</v>
       </c>
       <c r="B8">
@@ -1311,7 +1312,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9">
@@ -1331,7 +1332,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10">
@@ -1351,7 +1352,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>1609580427</v>
       </c>
       <c r="B11">
@@ -1371,7 +1372,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12">
@@ -1391,7 +1392,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B13">
@@ -1411,7 +1412,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B14">
@@ -1431,7 +1432,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B15">
@@ -1451,7 +1452,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>1938298071</v>
       </c>
       <c r="B16">
@@ -1471,7 +1472,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B17">
@@ -1491,7 +1492,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18">
@@ -1511,7 +1512,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>1423133080</v>
       </c>
       <c r="B19">
@@ -1531,7 +1532,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>1554537045</v>
       </c>
       <c r="B20">
@@ -1551,7 +1552,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>1465414053</v>
       </c>
       <c r="B21">
@@ -1571,7 +1572,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B22">
@@ -1591,7 +1592,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B23">
@@ -1611,7 +1612,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B24">
@@ -1631,7 +1632,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>1493527487</v>
       </c>
       <c r="B25">
@@ -1651,7 +1652,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B26">
@@ -1671,7 +1672,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B27">
@@ -1691,7 +1692,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B28">
@@ -1711,7 +1712,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B29">
@@ -1731,7 +1732,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B30">
@@ -1751,7 +1752,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B31">
@@ -1771,7 +1772,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B32">
@@ -1791,7 +1792,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B33">
@@ -1811,7 +1812,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B34">
@@ -1831,7 +1832,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B35">
@@ -1851,7 +1852,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>1442429771</v>
       </c>
       <c r="B36">
@@ -1871,7 +1872,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>1452109206</v>
       </c>
       <c r="B37">
@@ -1891,7 +1892,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B38">
@@ -1911,7 +1912,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B39">
@@ -1931,7 +1932,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B40">
@@ -1951,7 +1952,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B41">
@@ -1971,7 +1972,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B42">
@@ -1991,7 +1992,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>1416980067</v>
       </c>
       <c r="B43">
@@ -2011,7 +2012,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B44">
@@ -2031,7 +2032,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B45">
@@ -2051,7 +2052,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B46">
@@ -2071,7 +2072,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B47">
@@ -2091,7 +2092,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B48">
@@ -2111,7 +2112,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B49">
@@ -2131,7 +2132,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B50">
@@ -2151,7 +2152,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B51">
@@ -2171,7 +2172,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B52">
@@ -2191,7 +2192,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B53">
@@ -2211,7 +2212,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B54">
@@ -2231,7 +2232,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B55">
@@ -2251,7 +2252,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B56">
@@ -2271,7 +2272,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>1481466224</v>
       </c>
       <c r="B57">
@@ -2291,7 +2292,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B58">
@@ -2311,7 +2312,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B59">
@@ -2331,7 +2332,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B60">
@@ -2351,7 +2352,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B61">
@@ -2371,7 +2372,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B62">
@@ -2391,7 +2392,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B63">
@@ -2411,7 +2412,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B64">
@@ -2431,7 +2432,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B65">
@@ -2451,7 +2452,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B66">
@@ -2471,7 +2472,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B67">
@@ -2491,7 +2492,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B68">
@@ -2511,7 +2512,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B69">
@@ -2531,7 +2532,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B70">
@@ -2551,7 +2552,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B71">
@@ -2571,7 +2572,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B72">
@@ -2591,7 +2592,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>1477826351</v>
       </c>
       <c r="B73">
@@ -2611,7 +2612,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B74">
@@ -2631,7 +2632,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B75">
@@ -2651,7 +2652,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>1494430533</v>
       </c>
       <c r="B76">
@@ -2671,7 +2672,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B77">
@@ -2691,7 +2692,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>1423166310</v>
       </c>
       <c r="B78">
@@ -2711,7 +2712,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B79">
@@ -2731,7 +2732,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B80">
@@ -2751,7 +2752,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B81">
@@ -2771,7 +2772,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B82">
@@ -2791,7 +2792,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B83">
@@ -2811,7 +2812,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B84">
@@ -2831,7 +2832,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B85">
@@ -2851,7 +2852,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B86">
@@ -2871,7 +2872,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B87">
@@ -2891,7 +2892,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B88">
@@ -2911,7 +2912,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B89">
@@ -2931,7 +2932,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B90">
@@ -2951,7 +2952,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B91">
@@ -2971,7 +2972,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B92">
@@ -2991,7 +2992,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B93">
@@ -3011,7 +3012,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B94">
@@ -3031,7 +3032,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B95">
@@ -3051,7 +3052,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>1491524081</v>
       </c>
       <c r="B96">
@@ -3071,7 +3072,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B97">
@@ -3091,7 +3092,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B98">
@@ -3111,7 +3112,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B99">
@@ -3131,7 +3132,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>1442373636</v>
       </c>
       <c r="B100">
@@ -3151,7 +3152,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B101">
@@ -3171,7 +3172,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="A102" s="1">
         <v>1442360712</v>
       </c>
       <c r="B102">
@@ -3191,7 +3192,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="A103" s="1">
         <v>9657141591</v>
       </c>
       <c r="B103">
@@ -3211,7 +3212,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B104">
@@ -3231,7 +3232,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="A105" s="1">
         <v>1442354755</v>
       </c>
       <c r="B105">
@@ -3251,7 +3252,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B106">
@@ -3271,7 +3272,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B107">
@@ -3291,7 +3292,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B108">
@@ -3311,7 +3312,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B109">
@@ -3331,7 +3332,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B110">
@@ -3351,7 +3352,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>200</v>
       </c>
       <c r="B111">
@@ -3371,7 +3372,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B112">
@@ -3391,7 +3392,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B113">
@@ -3411,7 +3412,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="A114" s="1">
         <v>1481918087</v>
       </c>
       <c r="B114">
@@ -3431,7 +3432,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B115">
@@ -3451,7 +3452,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B116">
@@ -3471,7 +3472,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="A117" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B117">
@@ -3491,7 +3492,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B118">
@@ -3511,7 +3512,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="A119" s="1">
         <v>1442352965</v>
       </c>
       <c r="B119">
@@ -3531,7 +3532,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B120">
@@ -3551,7 +3552,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B121">
@@ -3571,7 +3572,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B122">
@@ -3591,7 +3592,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B123">
@@ -3611,7 +3612,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B124">
@@ -3631,7 +3632,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B125">
@@ -3651,7 +3652,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B126">
@@ -3671,7 +3672,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B127">
@@ -3691,7 +3692,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B128">
@@ -3711,7 +3712,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B129">

</xml_diff>